<commit_message>
Tweaked absolute refs and added named ranges
</commit_message>
<xml_diff>
--- a/metro_budget_worked.xlsx
+++ b/metro_budget_worked.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jcool\workspace\excel\data\metro_budget\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E68C930-AEC4-4372-826A-D72575A4BE17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82168CC9-7E30-44CD-BD3D-606A2A9057B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1141,8 +1141,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="H55" sqref="H55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3054,11 +3054,11 @@
         <v>-36209.629999999903</v>
       </c>
       <c r="C56">
-        <f>INDEX(dataset,MATCH($A56,AllDepartments,0), MATCH(C$55,Headers,0))</f>
+        <f t="shared" ref="B56:D61" si="1">INDEX(dataset,MATCH($A56,AllDepartments,0), MATCH(C$55,Headers,0))</f>
         <v>-27292.159999999902</v>
       </c>
       <c r="D56">
-        <f>INDEX(dataset,MATCH($A56,AllDepartments,0), MATCH(D$55,Headers,0))</f>
+        <f t="shared" si="1"/>
         <v>-9181.0800000000108</v>
       </c>
       <c r="E56">
@@ -3079,15 +3079,15 @@
         <v>19</v>
       </c>
       <c r="B57">
-        <f>INDEX(dataset,MATCH($A57,AllDepartments,0), MATCH(B$55,Headers,0))</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C57">
-        <f>INDEX(dataset,MATCH($A57,AllDepartments,0), MATCH(C$55,Headers,0))</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D57">
-        <f>INDEX(dataset,MATCH($A57,AllDepartments,0), MATCH(D$55,Headers,0))</f>
+        <f t="shared" si="1"/>
         <v>-311228.08999999898</v>
       </c>
     </row>
@@ -3096,15 +3096,15 @@
         <v>26</v>
       </c>
       <c r="B58">
-        <f>INDEX(dataset,MATCH($A58,AllDepartments,0), MATCH(B$55,Headers,0))</f>
+        <f t="shared" si="1"/>
         <v>-149396.1</v>
       </c>
       <c r="C58">
-        <f>INDEX(dataset,MATCH($A58,AllDepartments,0), MATCH(C$55,Headers,0))</f>
+        <f t="shared" si="1"/>
         <v>-189254.05999999901</v>
       </c>
       <c r="D58">
-        <f>INDEX(dataset,MATCH($A58,AllDepartments,0), MATCH(D$55,Headers,0))</f>
+        <f t="shared" si="1"/>
         <v>-374962.91</v>
       </c>
     </row>
@@ -3113,15 +3113,15 @@
         <v>32</v>
       </c>
       <c r="B59">
-        <f>INDEX(dataset,MATCH($A59,AllDepartments,0), MATCH(B$55,Headers,0))</f>
+        <f t="shared" si="1"/>
         <v>-12230.809999999799</v>
       </c>
       <c r="C59">
-        <f>INDEX(dataset,MATCH($A59,AllDepartments,0), MATCH(C$55,Headers,0))</f>
+        <f t="shared" si="1"/>
         <v>-45485.579999999798</v>
       </c>
       <c r="D59">
-        <f>INDEX(dataset,MATCH($A59,AllDepartments,0), MATCH(D$55,Headers,0))</f>
+        <f t="shared" si="1"/>
         <v>-72.879999999888199</v>
       </c>
     </row>
@@ -3130,15 +3130,15 @@
         <v>33</v>
       </c>
       <c r="B60">
-        <f>INDEX(dataset,MATCH($A60,AllDepartments,0), MATCH(B$55,Headers,0))</f>
+        <f t="shared" si="1"/>
         <v>-4950.4699999999102</v>
       </c>
       <c r="C60">
-        <f>INDEX(dataset,MATCH($A60,AllDepartments,0), MATCH(C$55,Headers,0))</f>
+        <f t="shared" si="1"/>
         <v>-8005.79000000003</v>
       </c>
       <c r="D60">
-        <f>INDEX(dataset,MATCH($A60,AllDepartments,0), MATCH(D$55,Headers,0))</f>
+        <f t="shared" si="1"/>
         <v>-1724.8999999999601</v>
       </c>
     </row>
@@ -3147,15 +3147,15 @@
         <v>49</v>
       </c>
       <c r="B61">
-        <f>INDEX(dataset,MATCH($A61,AllDepartments,0), MATCH(B$55,Headers,0))</f>
+        <f t="shared" si="1"/>
         <v>-184239.79</v>
       </c>
       <c r="C61">
-        <f>INDEX(dataset,MATCH($A61,AllDepartments,0), MATCH(C$55,Headers,0))</f>
+        <f t="shared" si="1"/>
         <v>-133456.33000000101</v>
       </c>
       <c r="D61">
-        <f>INDEX(dataset,MATCH($A61,AllDepartments,0), MATCH(D$55,Headers,0))</f>
+        <f t="shared" si="1"/>
         <v>-82077.349999997707</v>
       </c>
     </row>

</xml_diff>

<commit_message>
minor touches after review
</commit_message>
<xml_diff>
--- a/metro_budget_worked.xlsx
+++ b/metro_budget_worked.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jcool\workspace\excel\data\metro_budget\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82168CC9-7E30-44CD-BD3D-606A2A9057B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{161BE8BF-802F-4919-B68D-5D1339ECCBB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1139,10 +1139,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K61"/>
+  <dimension ref="A1:K66"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="H55" sqref="H55"/>
+      <selection activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3157,6 +3157,24 @@
       <c r="D61">
         <f t="shared" si="1"/>
         <v>-82077.349999997707</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <f>ROW(E50)</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <f>COLUMN(I17)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A66" t="str">
+        <f>ADDRESS(ROW(C34),COLUMN(C34))</f>
+        <v>$C$34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>